<commit_message>
Documentation: Weekly Report - 3
</commit_message>
<xml_diff>
--- a/Documentation/Project Weekly Report - FHF - 2.xlsx
+++ b/Documentation/Project Weekly Report - FHF - 2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC852822-57A8-40CB-BC1A-63F80867DDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3539ED-EB7F-4AB2-88C4-F09148D8860B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wx" sheetId="1" r:id="rId1"/>
@@ -181,9 +181,6 @@
     <t>SEP490_G1</t>
   </si>
   <si>
-    <t>05/09/2022-11/09/2022</t>
-  </si>
-  <si>
     <t>All Team</t>
   </si>
   <si>
@@ -269,6 +266,9 @@
   </si>
   <si>
     <t>Confirm with Mentor</t>
+  </si>
+  <si>
+    <t>12/09/2022-18/09/2022</t>
   </si>
 </sst>
 </file>
@@ -732,26 +732,26 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="A31:E31"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="38.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="57.44140625" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="8.77734375" style="4"/>
+    <col min="1" max="1" width="6.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="57.42578125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -759,20 +759,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -789,146 +789,146 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>4</v>
       </c>
@@ -945,53 +945,53 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
@@ -1008,83 +1008,83 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>4</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>4</v>
       </c>
@@ -1101,35 +1101,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="9"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>

</xml_diff>